<commit_message>
added events and changed names
</commit_message>
<xml_diff>
--- a/Example Notebooks/calendar_upload_test.xlsx
+++ b/Example Notebooks/calendar_upload_test.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qubstudentcloud-my.sharepoint.com/personal/3053304_ads_qub_ac_uk/Documents/QUB/Teaching/Canvas Calendar Upload Script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Dingwall\Documents\github\qub_canvas_helper\qub_canvas_helper\Example Notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{22CA9EDB-9D68-4C54-B5DD-DE9BDB6E33C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AB27F3B-9C5C-4F50-AEE4-A2520E5EF538}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3D0F8D-37B7-4D96-964C-A6F754FEC16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8775" windowWidth="29040" windowHeight="15840" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHM1101" sheetId="19" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CHM1101'!$A$1:$L$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'CHM1101'!$A$1:$L$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CHM1101'!$A$1:$L$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'CHM1101'!$A$1:$L$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'CHM1101'!$2:$5</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="55">
   <si>
     <t>Module Timetable</t>
   </si>
@@ -190,17 +190,29 @@
     <t>28/11/2023</t>
   </si>
   <si>
-    <t>Notareal Person</t>
-  </si>
-  <si>
-    <t>Lecturer McLecturerFace</t>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>ASH/01/006</t>
+  </si>
+  <si>
+    <t>ASH/01/007</t>
+  </si>
+  <si>
+    <t>Prof R Woodward</t>
+  </si>
+  <si>
+    <t>Prof B Sharpless</t>
+  </si>
+  <si>
+    <t>Redox Chemistry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +307,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1162,29 +1180,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.08984375" customWidth="1"/>
-    <col min="7" max="7" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.08984375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1218,7 @@
       <c r="K1" s="70"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1226,7 +1244,7 @@
       <c r="K2" s="74"/>
       <c r="L2" s="75"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1252,7 +1270,7 @@
       <c r="K3" s="77"/>
       <c r="L3" s="78"/>
     </row>
-    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>9</v>
       </c>
@@ -1267,7 +1285,7 @@
       <c r="J4" s="69"/>
       <c r="K4" s="69"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1302,7 +1320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>8</v>
       </c>
@@ -1310,7 +1328,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="23">
-        <v>45610</v>
+        <v>45640</v>
       </c>
       <c r="D6" s="32">
         <v>0.375</v>
@@ -1318,10 +1336,12 @@
       <c r="E6" s="32">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>23</v>
@@ -1333,76 +1353,83 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="24">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
         <v>9</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="25">
-        <v>45610</v>
-      </c>
-      <c r="D7" s="33">
+      <c r="B7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="23">
+        <f>C6+7</f>
+        <v>45647</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0.375</v>
+      </c>
+      <c r="E7" s="32">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E7" s="33">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="24">
+      <c r="F7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="17">
+        <v>394</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>10</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="25">
-        <v>45617</v>
-      </c>
-      <c r="D8" s="33">
+      <c r="B8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="23">
+        <f>C7+7</f>
+        <v>45654</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0.375</v>
+      </c>
+      <c r="E8" s="32">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E8" s="33">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="17">
+        <v>395</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="25">
-        <v>45624</v>
+        <v>45640</v>
       </c>
       <c r="D9" s="33">
         <v>0.41666666666666669</v>
@@ -1425,235 +1452,237 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>10</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="25">
+        <v>45647</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
         <v>12</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="25">
+        <v>45654</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="21">
-        <v>45612</v>
-      </c>
-      <c r="D10" s="34">
+      <c r="C12" s="21">
+        <v>45642</v>
+      </c>
+      <c r="D12" s="34">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E12" s="34">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13" t="s">
+      <c r="F12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="28">
+        <v>253</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>13</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="21">
+        <v>45643</v>
+      </c>
+      <c r="D13" s="34">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E13" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="28">
-        <v>253</v>
-      </c>
-      <c r="K10" s="13" t="s">
+      <c r="J13" s="28">
+        <v>254</v>
+      </c>
+      <c r="K13" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="7" t="s">
+    <row r="14" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>14</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="21">
+        <v>45644</v>
+      </c>
+      <c r="D14" s="34">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E14" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="28">
+        <v>255</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="K12" s="36"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="50">
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="K16" s="36"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="50">
         <v>8</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C17" s="55">
         <v>45118</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D17" s="62">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E13" s="62">
+      <c r="E17" s="62">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F13" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="F17" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="37" t="s">
+      <c r="I17" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="51">
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="51">
         <v>8</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="56">
-        <v>45118</v>
-      </c>
-      <c r="D14" s="63">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E14" s="63">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="52">
-        <v>8</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="57">
-        <v>45180</v>
-      </c>
-      <c r="D15" s="64">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="E15" s="64">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="52">
-        <v>8</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="57">
-        <v>45180</v>
-      </c>
-      <c r="D16" s="64">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E16" s="64">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="53">
-        <v>8</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="58">
-        <v>45210</v>
-      </c>
-      <c r="D17" s="65">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E17" s="65">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F17" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="51">
-        <v>9</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="59" t="s">
-        <v>32</v>
+      <c r="C18" s="56">
+        <v>45118</v>
       </c>
       <c r="D18" s="63">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E18" s="63">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>29</v>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>1</v>
       </c>
       <c r="G18" s="41" t="s">
         <v>1</v>
@@ -1668,56 +1697,56 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="51">
-        <v>9</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="63">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E19" s="63">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="42" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="52">
+        <v>8</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="57">
+        <v>45180</v>
+      </c>
+      <c r="D19" s="64">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E19" s="64">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" s="40" t="s">
+      <c r="I19" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="52">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="60" t="s">
-        <v>33</v>
+      <c r="C20" s="57">
+        <v>45180</v>
       </c>
       <c r="D20" s="64">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E20" s="64">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F20" s="44" t="s">
-        <v>31</v>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>1</v>
       </c>
       <c r="G20" s="43" t="s">
         <v>1</v>
@@ -1732,88 +1761,88 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="52">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="53">
+        <v>8</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="58">
+        <v>45210</v>
+      </c>
+      <c r="D21" s="65">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E21" s="65">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="51">
         <v>9</v>
       </c>
-      <c r="B21" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="64">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E21" s="64">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="44" t="s">
+      <c r="B22" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="63">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E22" s="63">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="35" t="s">
+      <c r="I22" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="53">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="51">
         <v>9</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="61" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="65">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E22" s="65">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="51">
-        <v>10</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="59" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="63">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E23" s="63">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F23" s="40" t="s">
-        <v>1</v>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>1</v>
@@ -1828,53 +1857,53 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="51">
-        <v>10</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="63">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E24" s="63">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="42" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="52">
+        <v>9</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="64">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E24" s="64">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="40" t="s">
+      <c r="I24" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="52">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="60" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25" s="64">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E25" s="64">
-        <v>0.54166666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F25" s="35" t="s">
         <v>1</v>
@@ -1892,85 +1921,85 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="52">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="53">
+        <v>9</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="65">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E26" s="65">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="51">
         <v>10</v>
       </c>
-      <c r="B26" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="64">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E26" s="64">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G26" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26" s="44" t="s">
+      <c r="B27" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="63">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E27" s="63">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="35" t="s">
+      <c r="I27" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="53">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="51">
         <v>10</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="65">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E27" s="65">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F27" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="J27" s="45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="51">
-        <v>11</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="59" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D28" s="63">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E28" s="63">
-        <v>0.54166666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F28" s="40" t="s">
         <v>1</v>
@@ -1987,56 +2016,54 @@
       <c r="J28" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="51">
-        <v>11</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="63">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E29" s="63">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F29" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="42" t="s">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="52">
+        <v>10</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="64">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E29" s="64">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="J29" s="40" t="s">
+      <c r="I29" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="52">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="60" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D30" s="64">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E30" s="64">
-        <v>0.54166666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F30" s="35" t="s">
         <v>1</v>
@@ -2053,115 +2080,245 @@
       <c r="J30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="52">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="53">
+        <v>10</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="65">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E31" s="65">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="51">
         <v>11</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B32" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="63">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E32" s="63">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="51">
+        <v>11</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="63">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E33" s="63">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="52">
+        <v>11</v>
+      </c>
+      <c r="B34" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C34" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="64">
+      <c r="D34" s="64">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E34" s="64">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="52">
+        <v>11</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="64">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E31" s="64">
+      <c r="E35" s="64">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F31" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="H31" s="44" t="s">
+      <c r="F35" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="J31" s="35" t="s">
+      <c r="I35" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="54">
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="54">
         <v>11</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B36" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="58">
+      <c r="C36" s="58">
         <v>44938</v>
       </c>
-      <c r="D32" s="66">
+      <c r="D36" s="66">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E36" s="66">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F32" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32" s="48" t="s">
+      <c r="F36" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="J32" s="45" t="s">
+      <c r="I36" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="L32"/>
-    </row>
-    <row r="33" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="L33"/>
-    </row>
-    <row r="34" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="L34"/>
-    </row>
-    <row r="35" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="L35"/>
+      <c r="L36"/>
+    </row>
+    <row r="37" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="L37"/>
+    </row>
+    <row r="38" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="L39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L10" xr:uid="{8D1A3C72-B371-41FB-80CB-3F55554D1BF9}">
+  <autoFilter ref="A1:L12" xr:uid="{8D1A3C72-B371-41FB-80CB-3F55554D1BF9}">
     <filterColumn colId="0" showButton="0"/>
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="2" showButton="0"/>
@@ -2182,11 +2339,12 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:L3"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Time should be in the format 14:30" sqref="E6:E10 D6:D10" xr:uid="{4864DA18-976D-4B65-9A33-653882B0B714}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Time should be in the format 14:30" sqref="D6:E14" xr:uid="{4864DA18-976D-4B65-9A33-653882B0B714}">
       <formula1>"08:00, 09:00, 10:00, 11:00, 12:00, 13:00, 14:00, 15:00, 16:00, 17:00, 18:00"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B10" xr:uid="{389B26BE-1874-465F-B9CC-454077AEEEF7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B14" xr:uid="{389B26BE-1874-465F-B9CC-454077AEEEF7}">
       <formula1>"Monday, Tuesday, Wednesday, Thursday, Friday"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2205,12 +2363,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B124AA781744C5459DC7595D804177BB" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c5623c5dc3ef85ea3f01442bc8283c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2324,6 +2476,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617C60FB-438D-439C-B22E-06F5CD7793C3}">
   <ds:schemaRefs>
@@ -2333,15 +2491,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF445638-0D50-47A9-B2D4-C6C3D3E1987F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC6AF946-28F6-493B-9873-A762C84B1507}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2357,6 +2506,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF445638-0D50-47A9-B2D4-C6C3D3E1987F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{eaab77ea-b4a5-49e3-a1e8-d6dd23a1f286}" enabled="0" method="" siteId="{eaab77ea-b4a5-49e3-a1e8-d6dd23a1f286}" removed="1"/>

</xml_diff>